<commit_message>
added smoke tag to actions scenario
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testData.xlsx
+++ b/src/test/resources/testData/testData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l-nar\Documents\YFrameworkFinalC6P\src\test\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orkar\IdeaProjects\YFrameworkFinalC12\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0344AC20-31A5-4A84-8093-4B84A3AC01F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E12DA1F-561E-4E73-9672-2060B2F8C4A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FAFC4DB7-22AD-4538-A979-73DF204759A3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="13">
   <si>
     <t>Amount</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>SDET</t>
+  </si>
+  <si>
+    <t>Ice Cream</t>
   </si>
 </sst>
 </file>
@@ -440,16 +443,16 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.140625" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" customWidth="1"/>
   </cols>
@@ -617,7 +620,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4">
         <v>44579</v>

</xml_diff>